<commit_message>
Works till parameter estimation Nov 13
</commit_message>
<xml_diff>
--- a/KineticModel/N2m_test.xlsx
+++ b/KineticModel/N2m_test.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -96,12 +97,6 @@
     <t>Metab</t>
   </si>
   <si>
-    <t>Mclow (mM)</t>
-  </si>
-  <si>
-    <t>Mchigh (mM)</t>
-  </si>
-  <si>
     <t>v2</t>
   </si>
   <si>
@@ -222,7 +217,13 @@
     <t>F[c]</t>
   </si>
   <si>
-    <t>[c] : 0.33 B + 0.33 C + 0.33 D ---&gt; F</t>
+    <t>[c] : B ---&gt; F</t>
+  </si>
+  <si>
+    <t>Mclow (M)</t>
+  </si>
+  <si>
+    <t>Mchigh (M)</t>
   </si>
 </sst>
 </file>
@@ -596,7 +597,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,18 +670,18 @@
         <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E2">
         <v>-8</v>
@@ -692,21 +693,21 @@
         <v>20</v>
       </c>
       <c r="S2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T2">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="U2">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E3">
         <v>-8</v>
@@ -718,21 +719,21 @@
         <v>20</v>
       </c>
       <c r="S3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T3">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="U3">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>-8</v>
@@ -744,21 +745,21 @@
         <v>20</v>
       </c>
       <c r="S4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="T4">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="U4">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -770,21 +771,21 @@
         <v>-40</v>
       </c>
       <c r="S5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T5">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="U5">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E6">
         <v>-8</v>
@@ -796,21 +797,21 @@
         <v>20</v>
       </c>
       <c r="S6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="T6">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="U6">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7">
         <v>-8</v>
@@ -822,21 +823,21 @@
         <v>20</v>
       </c>
       <c r="S7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="T7">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="U7">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -848,21 +849,21 @@
         <v>-10</v>
       </c>
       <c r="S8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T8">
-        <v>0.1</v>
+        <v>1E-4</v>
       </c>
       <c r="U8">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -879,10 +880,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -899,10 +900,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -919,10 +920,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -934,15 +935,15 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -953,38 +954,38 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -995,30 +996,30 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reset changes to callODESolver to use SUNDIALS instead of ode15s
</commit_message>
<xml_diff>
--- a/KineticModel/N2m_test.xlsx
+++ b/KineticModel/N2m_test.xlsx
@@ -16,12 +16,12 @@
     <sheet name="N2mOpen" sheetId="2" r:id="rId2"/>
     <sheet name="N2mClose" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="79">
   <si>
     <t>Enzymes</t>
   </si>
@@ -242,9 +242,6 @@
     <t>v10</t>
   </si>
   <si>
-    <t>[c] : C ---&gt; B</t>
-  </si>
-  <si>
     <t>v11</t>
   </si>
   <si>
@@ -276,6 +273,12 @@
   </si>
   <si>
     <t>E[c] ---&gt; E[e]</t>
+  </si>
+  <si>
+    <t>[c] : A ---&gt; D</t>
+  </si>
+  <si>
+    <t>[c] : C + D ---&gt; P + E</t>
   </si>
 </sst>
 </file>
@@ -652,7 +655,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1090,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,7 +1220,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -1243,7 +1246,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="E5">
         <v>-8</v>
@@ -1295,7 +1298,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="E7">
         <v>10</v>
@@ -1332,7 +1335,7 @@
         <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1343,7 +1346,7 @@
         <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1354,7 +1357,7 @@
         <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1362,34 +1365,34 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
         <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
         <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
         <v>73</v>
-      </c>
-      <c r="C15" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1402,7 +1405,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1532,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -1555,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="E5">
         <v>-8</v>
@@ -1607,7 +1610,7 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="E7">
         <v>10</v>

</xml_diff>